<commit_message>
new script for 2015
</commit_message>
<xml_diff>
--- a/2015_Bombus_Survey/RawData/SpatDatBuffs.xlsx
+++ b/2015_Bombus_Survey/RawData/SpatDatBuffs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipburnham/AlgerProjects/2015_Bombus_Survey/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,15 @@
     <sheet name="4km" sheetId="6" r:id="rId7"/>
     <sheet name="5km" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4398" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4322" uniqueCount="166">
   <si>
     <t>site</t>
   </si>
@@ -534,7 +540,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -848,13 +854,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -916,7 +922,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -978,7 +984,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1040,7 +1046,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1065,23 +1071,23 @@
       <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s">
-        <v>121</v>
-      </c>
-      <c r="J4" t="s">
-        <v>121</v>
-      </c>
-      <c r="K4" t="s">
-        <v>121</v>
-      </c>
-      <c r="L4" t="s">
-        <v>121</v>
-      </c>
-      <c r="M4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N4" t="s">
-        <v>121</v>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -1102,7 +1108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1375,17 +1381,17 @@
       <c r="H9" t="s">
         <v>33</v>
       </c>
-      <c r="I9" t="s">
-        <v>121</v>
-      </c>
-      <c r="J9" t="s">
-        <v>121</v>
-      </c>
-      <c r="K9" t="s">
-        <v>121</v>
-      </c>
-      <c r="L9" t="s">
-        <v>121</v>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -1412,7 +1418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1437,17 +1443,17 @@
       <c r="H10" t="s">
         <v>37</v>
       </c>
-      <c r="I10" t="s">
-        <v>121</v>
-      </c>
-      <c r="J10" t="s">
-        <v>121</v>
-      </c>
-      <c r="K10" t="s">
-        <v>121</v>
-      </c>
-      <c r="L10" t="s">
-        <v>121</v>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
       </c>
       <c r="M10">
         <v>3</v>
@@ -1474,7 +1480,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1499,23 +1505,23 @@
       <c r="H11" t="s">
         <v>39</v>
       </c>
-      <c r="I11" t="s">
-        <v>121</v>
-      </c>
-      <c r="J11" t="s">
-        <v>121</v>
-      </c>
-      <c r="K11" t="s">
-        <v>121</v>
-      </c>
-      <c r="L11" t="s">
-        <v>121</v>
-      </c>
-      <c r="M11" t="s">
-        <v>121</v>
-      </c>
-      <c r="N11" t="s">
-        <v>121</v>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
       </c>
       <c r="O11">
         <v>4</v>
@@ -1536,7 +1542,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1598,7 +1604,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1623,11 +1629,11 @@
       <c r="H13" t="s">
         <v>44</v>
       </c>
-      <c r="I13" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" t="s">
-        <v>121</v>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1660,7 +1666,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1685,35 +1691,35 @@
       <c r="H14" t="s">
         <v>47</v>
       </c>
-      <c r="I14" t="s">
-        <v>121</v>
-      </c>
-      <c r="J14" t="s">
-        <v>121</v>
-      </c>
-      <c r="K14" t="s">
-        <v>121</v>
-      </c>
-      <c r="L14" t="s">
-        <v>121</v>
-      </c>
-      <c r="M14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N14" t="s">
-        <v>121</v>
-      </c>
-      <c r="O14" t="s">
-        <v>121</v>
-      </c>
-      <c r="P14" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>121</v>
-      </c>
-      <c r="R14" t="s">
-        <v>121</v>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
       </c>
       <c r="S14">
         <v>1</v>
@@ -1722,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1747,44 +1753,44 @@
       <c r="H15" t="s">
         <v>50</v>
       </c>
-      <c r="I15" t="s">
-        <v>121</v>
-      </c>
-      <c r="J15" t="s">
-        <v>121</v>
-      </c>
-      <c r="K15" t="s">
-        <v>121</v>
-      </c>
-      <c r="L15" t="s">
-        <v>121</v>
-      </c>
-      <c r="M15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N15" t="s">
-        <v>121</v>
-      </c>
-      <c r="O15" t="s">
-        <v>121</v>
-      </c>
-      <c r="P15" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>121</v>
-      </c>
-      <c r="R15" t="s">
-        <v>121</v>
-      </c>
-      <c r="S15" t="s">
-        <v>121</v>
-      </c>
-      <c r="T15" t="s">
-        <v>121</v>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1809,11 +1815,11 @@
       <c r="H16" t="s">
         <v>53</v>
       </c>
-      <c r="I16" t="s">
-        <v>121</v>
-      </c>
-      <c r="J16" t="s">
-        <v>121</v>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1846,7 +1852,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1871,29 +1877,29 @@
       <c r="H17" t="s">
         <v>56</v>
       </c>
-      <c r="I17" t="s">
-        <v>121</v>
-      </c>
-      <c r="J17" t="s">
-        <v>121</v>
-      </c>
-      <c r="K17" t="s">
-        <v>121</v>
-      </c>
-      <c r="L17" t="s">
-        <v>121</v>
-      </c>
-      <c r="M17" t="s">
-        <v>121</v>
-      </c>
-      <c r="N17" t="s">
-        <v>121</v>
-      </c>
-      <c r="O17" t="s">
-        <v>121</v>
-      </c>
-      <c r="P17" t="s">
-        <v>121</v>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
       </c>
       <c r="Q17">
         <v>2</v>
@@ -1908,7 +1914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1933,35 +1939,35 @@
       <c r="H18" t="s">
         <v>59</v>
       </c>
-      <c r="I18" t="s">
-        <v>121</v>
-      </c>
-      <c r="J18" t="s">
-        <v>121</v>
-      </c>
-      <c r="K18" t="s">
-        <v>121</v>
-      </c>
-      <c r="L18" t="s">
-        <v>121</v>
-      </c>
-      <c r="M18" t="s">
-        <v>121</v>
-      </c>
-      <c r="N18" t="s">
-        <v>121</v>
-      </c>
-      <c r="O18" t="s">
-        <v>121</v>
-      </c>
-      <c r="P18" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>121</v>
-      </c>
-      <c r="R18" t="s">
-        <v>121</v>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
       </c>
       <c r="S18">
         <v>3</v>
@@ -1970,7 +1976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -1995,29 +2001,29 @@
       <c r="H19" t="s">
         <v>62</v>
       </c>
-      <c r="I19" t="s">
-        <v>121</v>
-      </c>
-      <c r="J19" t="s">
-        <v>121</v>
-      </c>
-      <c r="K19" t="s">
-        <v>121</v>
-      </c>
-      <c r="L19" t="s">
-        <v>121</v>
-      </c>
-      <c r="M19" t="s">
-        <v>121</v>
-      </c>
-      <c r="N19" t="s">
-        <v>121</v>
-      </c>
-      <c r="O19" t="s">
-        <v>121</v>
-      </c>
-      <c r="P19" t="s">
-        <v>121</v>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
       </c>
       <c r="Q19">
         <v>3</v>
@@ -2032,7 +2038,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -2057,17 +2063,17 @@
       <c r="H20" t="s">
         <v>65</v>
       </c>
-      <c r="I20" t="s">
-        <v>121</v>
-      </c>
-      <c r="J20" t="s">
-        <v>121</v>
-      </c>
-      <c r="K20" t="s">
-        <v>121</v>
-      </c>
-      <c r="L20" t="s">
-        <v>121</v>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
       </c>
       <c r="M20">
         <v>2</v>
@@ -2104,13 +2110,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -2202,7 +2208,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2294,7 +2300,7 @@
         <v>7.9567100000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2386,7 +2392,7 @@
         <v>5.6134380000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2478,7 +2484,7 @@
         <v>2253.9647500000001</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2570,7 +2576,7 @@
         <v>1.8439639999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2662,7 +2668,7 @@
         <v>6.1157279999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2754,7 +2760,7 @@
         <v>13.226067</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2846,7 +2852,7 @@
         <v>12.226276</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2938,7 +2944,7 @@
         <v>1299.397252</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3030,7 +3036,7 @@
         <v>1107.8255489999999</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3122,7 +3128,7 @@
         <v>2007.7121509999999</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3214,7 +3220,7 @@
         <v>4.7569679999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3306,7 +3312,7 @@
         <v>991.57773999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3398,7 +3404,7 @@
         <v>4749.1004329999996</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>7209.6228419999998</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3582,7 +3588,7 @@
         <v>874.17285300000003</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3674,7 +3680,7 @@
         <v>3610.3081440000001</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3766,7 +3772,7 @@
         <v>4624.4250350000002</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3858,7 +3864,7 @@
         <v>3000.3082490000002</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3963,12 +3969,12 @@
       <selection activeCell="AJ23" sqref="AJ23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="37" max="37" width="27.28515625" customWidth="1"/>
+    <col min="37" max="37" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4129,7 +4135,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4290,7 +4296,7 @@
         <v>2010619.0746879999</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4451,7 +4457,7 @@
         <v>2010619.2558869999</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4612,7 +4618,7 @@
         <v>2010619.231648</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4773,7 +4779,7 @@
         <v>2010619.549083</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4934,7 +4940,7 @@
         <v>2010619.4720610001</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5095,7 +5101,7 @@
         <v>2010619.417041</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5256,7 +5262,7 @@
         <v>2010619.318122</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5417,7 +5423,7 @@
         <v>2010619.547583</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5578,7 +5584,7 @@
         <v>2010619.362559</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5739,7 +5745,7 @@
         <v>2010619.329437</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5900,7 +5906,7 @@
         <v>2010619.2168340001</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6061,7 +6067,7 @@
         <v>2010619.210371</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6222,7 +6228,7 @@
         <v>2010619.439793</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6383,7 +6389,7 @@
         <v>2010619.226452</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6544,7 +6550,7 @@
         <v>2010619.4448470001</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6705,7 +6711,7 @@
         <v>2010619.450804</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6866,7 +6872,7 @@
         <v>2010619.0556940001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -7027,7 +7033,7 @@
         <v>2010619.2738419999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -7201,12 +7207,12 @@
       <selection activeCell="AM2" sqref="AM2:AM20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="39" max="39" width="22.85546875" customWidth="1"/>
+    <col min="39" max="39" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -7373,7 +7379,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7540,7 +7546,7 @@
         <v>3141592.3740770002</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7707,7 +7713,7 @@
         <v>3141592.6005770001</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7874,7 +7880,7 @@
         <v>3141592.5702780001</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8041,7 +8047,7 @@
         <v>3141592.967071</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8208,7 +8214,7 @@
         <v>3141592.8707949999</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8375,7 +8381,7 @@
         <v>3141592.8020190001</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8542,7 +8548,7 @@
         <v>3141592.6783710001</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -8709,7 +8715,7 @@
         <v>3141592.9651959999</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -8876,7 +8882,7 @@
         <v>3141592.733916</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9043,7 +9049,7 @@
         <v>3141592.692514</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9210,7 +9216,7 @@
         <v>3141592.551761</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -9377,7 +9383,7 @@
         <v>3141592.5436820001</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9544,7 +9550,7 @@
         <v>3141592.8304599999</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9711,7 +9717,7 @@
         <v>3141592.5637830002</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -9878,7 +9884,7 @@
         <v>3141592.8367770002</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10045,7 +10051,7 @@
         <v>3141592.8442230001</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10212,7 +10218,7 @@
         <v>3141592.3503359999</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10379,7 +10385,7 @@
         <v>3141592.6230210001</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10559,12 +10565,12 @@
       <selection activeCell="AM2" sqref="AM2:AM20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="39" max="39" width="24.7109375" customWidth="1"/>
+    <col min="39" max="39" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -10731,7 +10737,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10898,7 +10904,7 @@
         <v>12566370.055334</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11065,7 +11071,7 @@
         <v>12566370.508334</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11232,7 +11238,7 @@
         <v>12566370.447736001</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11399,7 +11405,7 @@
         <v>12566371.241322</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11566,7 +11572,7 @@
         <v>12566371.048769001</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11733,7 +11739,7 @@
         <v>12566370.911217</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11900,7 +11906,7 @@
         <v>12566370.663921</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12067,7 +12073,7 @@
         <v>12566371.237571999</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -12234,7 +12240,7 @@
         <v>12566370.775012</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -12401,7 +12407,7 @@
         <v>12566370.692208</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -12568,7 +12574,7 @@
         <v>12566370.410700999</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -12735,7 +12741,7 @@
         <v>12566370.394544</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -12902,7 +12908,7 @@
         <v>12566370.968099</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -13069,7 +13075,7 @@
         <v>12566370.434746001</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -13236,7 +13242,7 @@
         <v>12566370.980733</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -13403,7 +13409,7 @@
         <v>12566370.995625</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -13570,7 +13576,7 @@
         <v>12566370.007851999</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -13737,7 +13743,7 @@
         <v>12566370.553222001</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -13917,12 +13923,12 @@
       <selection activeCell="AM2" sqref="AM2:AM20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="39" max="39" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -14089,7 +14095,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -14256,7 +14262,7 @@
         <v>28274333.043770999</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -14423,7 +14429,7 @@
         <v>28274333.723271001</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -14590,7 +14596,7 @@
         <v>28274333.632374</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -14757,7 +14763,7 @@
         <v>28274334.822753001</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -14924,7 +14930,7 @@
         <v>28274334.533923</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -15091,7 +15097,7 @@
         <v>28274334.327596001</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -15258,7 +15264,7 @@
         <v>28274333.95665</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -15425,7 +15431,7 @@
         <v>28274334.817127001</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -15592,7 +15598,7 @@
         <v>28274334.123287</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -15759,7 +15765,7 @@
         <v>28274333.999081001</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -15926,7 +15932,7 @@
         <v>28274333.576820999</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -16093,7 +16099,7 @@
         <v>28274333.552584998</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -16260,7 +16266,7 @@
         <v>28274334.412916999</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -16427,7 +16433,7 @@
         <v>28274333.612888001</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -16594,7 +16600,7 @@
         <v>28274334.431869</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -16761,7 +16767,7 @@
         <v>28274334.454206999</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -16928,7 +16934,7 @@
         <v>28274332.972546998</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -17095,7 +17101,7 @@
         <v>28274333.790601999</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -17275,12 +17281,12 @@
       <selection activeCell="AM2" sqref="AM2:AM20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="39" max="39" width="24.42578125" customWidth="1"/>
+    <col min="39" max="39" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -17447,7 +17453,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17614,7 +17620,7 @@
         <v>50265481.339387</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -17781,7 +17787,7 @@
         <v>50265482.245387003</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -17948,7 +17954,7 @@
         <v>50265482.124191001</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -18115,7 +18121,7 @@
         <v>50265483.711363003</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -18282,7 +18288,7 @@
         <v>50265483.326256</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -18449,7 +18455,7 @@
         <v>50265483.051152997</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -18616,7 +18622,7 @@
         <v>50265482.556560002</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -18783,7 +18789,7 @@
         <v>50265483.703861997</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -18950,7 +18956,7 @@
         <v>50265482.778742999</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -19117,7 +19123,7 @@
         <v>50265482.613133997</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -19284,7 +19290,7 @@
         <v>50265482.050121002</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -19451,7 +19457,7 @@
         <v>50265482.017806001</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -19618,7 +19624,7 @@
         <v>50265483.164916001</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -19785,7 +19791,7 @@
         <v>50265482.09821</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -19952,7 +19958,7 @@
         <v>50265483.190185003</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -20119,7 +20125,7 @@
         <v>50265483.219967999</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -20286,7 +20292,7 @@
         <v>50265481.244422004</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -20453,7 +20459,7 @@
         <v>50265482.335161999</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -20630,12 +20636,12 @@
   <dimension ref="A1:BC20"/>
   <sheetViews>
     <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2:AM20"/>
+      <selection activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -20802,7 +20808,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -20969,7 +20975,7 @@
         <v>78539814.942183003</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -21136,7 +21142,7 @@
         <v>78539816.074681997</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -21303,7 +21309,7 @@
         <v>78539815.923187003</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -21470,7 +21476,7 @@
         <v>78539817.907152995</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -21637,7 +21643,7 @@
         <v>78539817.425769001</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -21804,7 +21810,7 @@
         <v>78539817.081890002</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -21971,7 +21977,7 @@
         <v>78539816.463648006</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -22138,7 +22144,7 @@
         <v>78539817.897775993</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -22305,7 +22311,7 @@
         <v>78539816.741376996</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -22472,7 +22478,7 @@
         <v>78539816.534365997</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -22639,7 +22645,7 @@
         <v>78539815.830599993</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -22806,7 +22812,7 @@
         <v>78539815.790206</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -22973,7 +22979,7 @@
         <v>78539817.224093005</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -23140,7 +23146,7 @@
         <v>78539815.890710995</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -23307,7 +23313,7 @@
         <v>78539817.255679995</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -23474,7 +23480,7 @@
         <v>78539817.292908996</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -23641,7 +23647,7 @@
         <v>78539814.823476002</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -23808,7 +23814,7 @@
         <v>78539816.186901003</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>

</xml_diff>